<commit_message>
correction bug du excel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>ID</t>
   </si>
@@ -41,7 +41,13 @@
     <t>En cours</t>
   </si>
   <si>
+    <t>2025-02-05</t>
+  </si>
+  <si>
     <t>Carte bancaire</t>
+  </si>
+  <si>
+    <t>cash</t>
   </si>
 </sst>
 </file>
@@ -134,7 +140,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,8 +201,37 @@
       <c r="F2" t="s" s="0">
         <v>8</v>
       </c>
+      <c r="G2" t="s" s="0">
+        <v>9</v>
+      </c>
       <c r="H2" t="s" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C3" t="n" s="0">
+        <v>2025.0</v>
+      </c>
+      <c r="D3" t="n" s="0">
+        <v>100000.0</v>
+      </c>
+      <c r="E3" t="n" s="0">
+        <v>10.0</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s" s="0">
         <v>9</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixation des bugs apres merge avec lampadaires intelligentes
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -187,7 +187,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="C2" t="n" s="0">
         <v>2025.0</v>
@@ -213,7 +213,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>1.0</v>
+        <v>9.0</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>2025.0</v>

</xml_diff>

<commit_message>
integration avec gestion utilisateur et fixation des interfaces
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -187,7 +187,7 @@
         <v>1.0</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="C2" t="n" s="0">
         <v>2025.0</v>
@@ -213,7 +213,7 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="C3" t="n" s="0">
         <v>2025.0</v>

</xml_diff>